<commit_message>
Issue no. 70 @1418675072
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -104,6 +104,33 @@
   </si>
   <si>
     <t>dial line on BodySun@baseline cut by fov</t>
+  </si>
+  <si>
+    <t>CircleParallel</t>
+  </si>
+  <si>
+    <t>circle inside fov</t>
+  </si>
+  <si>
+    <t>circle cut by fov</t>
+  </si>
+  <si>
+    <t>DialDeg</t>
+  </si>
+  <si>
+    <t>dial rail on CircleParallel inside fov</t>
+  </si>
+  <si>
+    <t>dial rail on CircleParallel cut by fov</t>
+  </si>
+  <si>
+    <t>CircleMeridian</t>
+  </si>
+  <si>
+    <t>dial rail on CircleMeridian inside fov</t>
+  </si>
+  <si>
+    <t>dial rail on CircleMeridian cut by fov</t>
   </si>
 </sst>
 </file>
@@ -468,7 +495,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +559,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E23" si="0">"tf-"&amp;TEXT(A3,"0000")&amp;".xml"</f>
+        <f t="shared" ref="E3:E30" si="0">"tf-"&amp;TEXT(A3,"0000")&amp;".xml"</f>
         <v>tf-0002.xml</v>
       </c>
     </row>
@@ -825,40 +852,120 @@
       <c r="A23" s="3">
         <v>22</v>
       </c>
+      <c r="B23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0022.xml</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
+      <c r="B24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0023.xml</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
+      <c r="B25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0024.xml</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
+      <c r="B26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0025.xml</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
+      <c r="B27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0026.xml</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
+      <c r="B28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0027.xml</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
+      <c r="B29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0028.xml</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0029.xml</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Issue no. 73 @1427830117
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="definition" sheetId="11" r:id="rId1"/>
+    <sheet name="set" sheetId="13" r:id="rId2"/>
+    <sheet name="file" sheetId="12" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>id</t>
   </si>
@@ -40,9 +42,6 @@
     <t>log</t>
   </si>
   <si>
-    <t>run</t>
-  </si>
-  <si>
     <t>element</t>
   </si>
   <si>
@@ -131,6 +130,57 @@
   </si>
   <si>
     <t>dial rail on CircleMeridian cut by fov</t>
+  </si>
+  <si>
+    <t>ChartAzimuthal</t>
+  </si>
+  <si>
+    <t>set pref node Artwork/ key dpi to value 36.</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>../stellarium/0.12/skycultures/western/andromeda.png</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>sf-ADC1239-popper-AND.dat</t>
+  </si>
+  <si>
+    <t>lib/cat/5050/catalog.dat.gz</t>
+  </si>
+  <si>
+    <t>stereographic northern star chart</t>
+  </si>
+  <si>
+    <t>stereographic southern star chart</t>
+  </si>
+  <si>
+    <t>orthographic northern star chart</t>
+  </si>
+  <si>
+    <t>orthographic southern star chart</t>
+  </si>
+  <si>
+    <t>stereographic map Andromeda to heaven</t>
+  </si>
+  <si>
+    <t>stereographic map Andromeda to projection plane</t>
+  </si>
+  <si>
+    <t>ChartPseudoCylindrical</t>
+  </si>
+  <si>
+    <t>Mollweide projection</t>
+  </si>
+  <si>
+    <t>Mollweide map Andromeda to heaven</t>
   </si>
 </sst>
 </file>
@@ -174,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -187,9 +237,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +552,7 @@
     <col min="3" max="3" width="38.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="60.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="5"/>
+    <col min="6" max="6" width="8.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="40.7109375" style="4" customWidth="1"/>
     <col min="8" max="16384" width="11.42578125" style="3"/>
   </cols>
@@ -515,19 +562,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>7</v>
@@ -559,7 +606,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E30" si="0">"tf-"&amp;TEXT(A3,"0000")&amp;".xml"</f>
+        <f t="shared" ref="E3:E38" si="0">"tf-"&amp;TEXT(A3,"0000")&amp;".xml"</f>
         <v>tf-0002.xml</v>
       </c>
     </row>
@@ -568,10 +615,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" si="0"/>
@@ -583,10 +630,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -598,10 +645,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -613,10 +660,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
@@ -658,10 +705,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -673,10 +720,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" si="0"/>
@@ -688,10 +735,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" si="0"/>
@@ -703,10 +750,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" si="0"/>
@@ -721,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -736,7 +783,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -748,243 +795,558 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0015.xml</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0016.xml</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0017.xml</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0018.xml</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0019.xml</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0020.xml</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0021.xml</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="E23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0022.xml</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0023.xml</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="E25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0024.xml</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0025.xml</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0026.xml</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0027.xml</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0028.xml</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tf-0029.xml</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0030.xml</v>
+      </c>
+      <c r="F31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0031.xml</v>
+      </c>
+      <c r="F32" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0032.xml</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0033.xml</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0034.xml</v>
+      </c>
+      <c r="F35" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0035.xml</v>
+      </c>
+      <c r="F36" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0036.xml</v>
+      </c>
+      <c r="F37" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>tf-0037.xml</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="60.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="60.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>